<commit_message>
Before using the code edit the config file
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/testdata/linkedLin_Credentials.xlsx
+++ b/src/main/java/com/crm/testdata/linkedLin_Credentials.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +118,61 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -163,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +229,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,6 +572,17 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -539,6 +616,39 @@
       <c r="J1" t="s" s="7">
         <v>20</v>
       </c>
+      <c r="K1" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s" s="11">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s" s="15">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s" s="17">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s" s="18">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -571,6 +681,39 @@
       <c r="J2" t="s">
         <v>21</v>
       </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -603,6 +746,39 @@
       <c r="J3" t="s">
         <v>21</v>
       </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -635,6 +811,39 @@
       <c r="J4" t="s">
         <v>21</v>
       </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -667,6 +876,39 @@
       <c r="J5" t="s">
         <v>21</v>
       </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -697,6 +939,39 @@
         <v>21</v>
       </c>
       <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U6" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Customize onClick function with Explictwait
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/testdata/linkedLin_Credentials.xlsx
+++ b/src/main/java/com/crm/testdata/linkedLin_Credentials.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +118,21 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -218,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,6 +255,9 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,6 +601,9 @@
     <col min="19" max="19" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -649,6 +670,15 @@
       <c r="U1" t="s" s="18">
         <v>20</v>
       </c>
+      <c r="V1" t="s" s="19">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s" s="20">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s" s="21">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -714,6 +744,15 @@
       <c r="U2" t="s">
         <v>21</v>
       </c>
+      <c r="V2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -779,6 +818,15 @@
       <c r="U3" t="s">
         <v>21</v>
       </c>
+      <c r="V3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -844,6 +892,15 @@
       <c r="U4" t="s">
         <v>21</v>
       </c>
+      <c r="V4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -909,6 +966,15 @@
       <c r="U5" t="s">
         <v>21</v>
       </c>
+      <c r="V5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" t="s">
+        <v>21</v>
+      </c>
+      <c r="X5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -972,6 +1038,15 @@
         <v>21</v>
       </c>
       <c r="U6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W6" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>